<commit_message>
Fixed attachment upload and updated test notebook Tricahue_XDC
</commit_message>
<xml_diff>
--- a/tests/test_files/Tricahue_v11.6b_Medias.xlsx
+++ b/tests/test_files/Tricahue_v11.6b_Medias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smf12\SPUR\Tricahue\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BA234F-6224-41EF-9D18-73D69D6D0B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2676EA6-AB9C-4202-AD1A-6CA42CFBE20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="1860" windowWidth="14400" windowHeight="8710" tabRatio="745" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7915" uniqueCount="7742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7918" uniqueCount="7745">
   <si>
     <t>Medias Metadata Template</t>
   </si>
@@ -23271,6 +23271,15 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>ExampleMedia</t>
+  </si>
+  <si>
+    <t>Example media</t>
+  </si>
+  <si>
+    <t>Upload example</t>
   </si>
 </sst>
 </file>
@@ -23376,7 +23385,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -23411,6 +23420,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor auto="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -23529,7 +23544,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -23566,6 +23581,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -23859,8 +23879,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1212" displayName="Table_1212" ref="A4:I7" totalsRowShown="0" dataDxfId="20">
-  <autoFilter ref="A4:I7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1212" displayName="Table_1212" ref="A4:I8" totalsRowShown="0" dataDxfId="20">
+  <autoFilter ref="A4:I8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Media ID" dataDxfId="19">
       <calculatedColumnFormula>IF(Table_1212[[#This Row],[Media Name]]=0,"",Table_1212[[#This Row],[Media Name]])</calculatedColumnFormula>
@@ -24493,7 +24513,7 @@
       </c>
       <c r="H6" t="str">
         <f>IF(Media!B8=0,"",Media!B8)</f>
-        <v/>
+        <v>Example media</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -33534,7 +33554,7 @@
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" t="str">
         <f>IF(Media!A8=0,"",Media!A8)</f>
-        <v/>
+        <v>ExampleMedia</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
@@ -36090,8 +36110,8 @@
   </sheetPr>
   <dimension ref="A1:L926"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -36214,7 +36234,25 @@
         <v>962</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>7742</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>7743</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>7744</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="28" t="e">
+        <f t="array" aca="1" ref="F8" ca="1">IsURL(Table_1212[[#This Row],[Data Source]])</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+    </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -37134,13 +37172,13 @@
     <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="B5:B7">
+  <conditionalFormatting sqref="B5:B8">
     <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>ISBLANK(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="The URL entered seems to be invalid, please check again." sqref="E5:E7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="The URL entered seems to be invalid, please check again." sqref="E5:E8" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>F5</formula1>
     </dataValidation>
   </dataValidations>
@@ -37398,7 +37436,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>